<commit_message>
A new attr.xlsx with Format:row 13 and Format:column D hidden
</commit_message>
<xml_diff>
--- a/files/attr.xlsx
+++ b/files/attr.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="17100" windowHeight="10365"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="17100" windowHeight="10365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Colours" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="39">
   <si>
     <t>red</t>
   </si>
@@ -110,6 +110,30 @@
   </si>
   <si>
     <t>hidden</t>
+  </si>
+  <si>
+    <t>Last row</t>
+  </si>
+  <si>
+    <t>Hidden row</t>
+  </si>
+  <si>
+    <t>Last Cell</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>column D</t>
+  </si>
+  <si>
+    <t>is hidden</t>
+  </si>
+  <si>
+    <t>Row 13 is hidden</t>
   </si>
 </sst>
 </file>
@@ -117,11 +141,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00_-"/>
-    <numFmt numFmtId="165" formatCode="d/m"/>
-    <numFmt numFmtId="166" formatCode="00.00.00.000"/>
-    <numFmt numFmtId="167" formatCode="**\ #,###,#00,000.00,**"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00_-"/>
+    <numFmt numFmtId="166" formatCode="d/m"/>
+    <numFmt numFmtId="167" formatCode="00.00.00.000"/>
+    <numFmt numFmtId="168" formatCode="**\ #,###,#00,000.00,**"/>
   </numFmts>
   <fonts count="50">
     <font>
@@ -474,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -655,16 +679,16 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -672,6 +696,10 @@
       <protection locked="0" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -968,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1245,32 +1273,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>12345</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="141">
         <v>12345</v>
       </c>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="155" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="154"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="155"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="142">
         <v>12345</v>
       </c>
@@ -1278,7 +1307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="143">
         <v>12345</v>
       </c>
@@ -1286,49 +1315,82 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="144">
         <v>12345</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="145">
         <v>12345</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="146">
         <v>12345</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="154" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="147">
         <v>12345</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="154" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="148">
         <v>12345</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="149">
         <v>12345</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="150">
         <v>12345</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" s="151">
         <v>12345</v>
       </c>
+      <c r="B12" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="156"/>
+    </row>
+    <row r="13" spans="1:5" hidden="1">
+      <c r="A13" s="154" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="154" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="154" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="154" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="154" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="154" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1529,7 +1591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="22.5">
       <c r="A4" s="101" t="s">
         <v>18</v>
       </c>

</xml_diff>